<commit_message>
working version with correct domain.yaml output
</commit_message>
<xml_diff>
--- a/xls2yaml/example/intent_action_table.xlsx
+++ b/xls2yaml/example/intent_action_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicoelbert/Documents/GitHub/unibot.tools/xls2yaml/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F85DB6-B7F6-AA40-8C86-F1139D526963}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE44D671-D0F7-F545-AA18-D54A14B121AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="73640" yWindow="0" windowWidth="23960" windowHeight="28800" xr2:uid="{A22D3741-E82E-A44C-BBEF-57F87B8EC504}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="222">
   <si>
     <t>intent</t>
   </si>
@@ -783,18 +783,6 @@
   <si>
     <t>Hallo
 Test</t>
-  </si>
-  <si>
-    <t>mensa/speiseplan</t>
-  </si>
-  <si>
-    <t>Was ist der aktuelle speiseplan</t>
-  </si>
-  <si>
-    <t>utter_mensa/speiseplan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das ist der speiseplan </t>
   </si>
 </sst>
 </file>
@@ -1389,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE1D935-0ED6-6046-98B9-0D2BD2DF12D7}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1606,14 +1594,6 @@
         <v>180</v>
       </c>
       <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>225</v>
-      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
@@ -1919,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BCC688-EC09-1B48-857C-F2BCC2698F65}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView topLeftCell="A88" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+      <selection activeCell="A131" sqref="A131:R133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3494,14 +3474,6 @@
         <v>faq/faq/residence_registration</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>222</v>
-      </c>
-      <c r="B131" t="s">
-        <v>223</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>